<commit_message>
updated BOM; minor formatting changes to SW proto
</commit_message>
<xml_diff>
--- a/Disk-O_BOM.xlsx
+++ b/Disk-O_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9564"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="9324"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>Adafruit</t>
   </si>
@@ -74,16 +74,13 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>1470-2282-ND</t>
-  </si>
-  <si>
     <t>Microcontroller dev board</t>
   </si>
   <si>
     <t xml:space="preserve">Teensy 3.1 32-bit ARM </t>
   </si>
   <si>
-    <t>1625</t>
+    <t>Sparkfun</t>
   </si>
   <si>
     <t>Prototyping board</t>
@@ -95,42 +92,124 @@
     <t>10k</t>
   </si>
   <si>
-    <t>Screw terminal #1</t>
-  </si>
-  <si>
-    <t>2-position 0.2"</t>
-  </si>
-  <si>
-    <t>Screw terminal #2</t>
-  </si>
-  <si>
-    <t>Resistor #1</t>
-  </si>
-  <si>
-    <t>Resistor #2</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>Power indicator LED</t>
   </si>
   <si>
-    <t xml:space="preserve">red </t>
-  </si>
-  <si>
     <t>Status LED</t>
   </si>
   <si>
-    <t>green</t>
+    <t>Miscellaneous wire</t>
+  </si>
+  <si>
+    <t>Screw terminal</t>
+  </si>
+  <si>
+    <t>4-position</t>
+  </si>
+  <si>
+    <t>Electrolytic cap</t>
+  </si>
+  <si>
+    <t>ED2582-ND</t>
+  </si>
+  <si>
+    <t>PRT-12070</t>
+  </si>
+  <si>
+    <t>DEV-13635</t>
+  </si>
+  <si>
+    <t>Female header</t>
+  </si>
+  <si>
+    <t>received 2</t>
+  </si>
+  <si>
+    <t>ordered 16 ft. 5/21/15</t>
+  </si>
+  <si>
+    <t>ordered 2 pcs. 5/21/15</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>ext. cost</t>
+  </si>
+  <si>
+    <t>ZVP2106A-ND</t>
+  </si>
+  <si>
+    <t>67-2063-ND</t>
+  </si>
+  <si>
+    <t>turquoise</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>67-2064-ND</t>
+  </si>
+  <si>
+    <t>Resistor #1 - level translation</t>
+  </si>
+  <si>
+    <t>Resistor #2 - power and status indicator</t>
+  </si>
+  <si>
+    <t>CF14JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>62 Ohm</t>
+  </si>
+  <si>
+    <t>CF14JT62R0CT-ND</t>
+  </si>
+  <si>
+    <t>1189-2570-ND</t>
+  </si>
+  <si>
+    <t>14-position</t>
+  </si>
+  <si>
+    <t>S7012-ND</t>
+  </si>
+  <si>
+    <t>M3 standoff</t>
+  </si>
+  <si>
+    <t>M3 screw</t>
+  </si>
+  <si>
+    <t>1470-2287-ND</t>
+  </si>
+  <si>
+    <t>Spade terminal</t>
+  </si>
+  <si>
+    <t>277-9649-ND</t>
+  </si>
+  <si>
+    <t>335-1156-ND</t>
+  </si>
+  <si>
+    <t>952-2311-ND</t>
+  </si>
+  <si>
+    <t>ordered 2 pcs. 5/22/15</t>
+  </si>
+  <si>
+    <t>ordered 3 pcs. 5/22/15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -170,12 +249,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,15 +537,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G16"/>
+  <dimension ref="A3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -481,14 +569,21 @@
       <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>134.94999999999999</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1">
+        <f>A4*F4</f>
+        <v>134.94999999999999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -504,14 +599,21 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>1.99</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H21" si="0">A5*F5</f>
+        <v>11.94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -527,136 +629,405 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>3.89</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5">
+        <v>19.95</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>19.95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1">
-        <v>19.95</v>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4.95</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <f>A9*F9</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1.22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="1">
+        <f>SUM(H4:H21)</f>
+        <v>215.39999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -664,10 +1035,22 @@
     <hyperlink ref="E4" r:id="rId1"/>
     <hyperlink ref="E5" r:id="rId2"/>
     <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E16" r:id="rId4"/>
     <hyperlink ref="E8" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E15" r:id="rId12"/>
+    <hyperlink ref="E17" r:id="rId13"/>
+    <hyperlink ref="E9" r:id="rId14" display="http://www.digikey.com/product-search/en?vendor=0&amp;keywords=VCS70US05"/>
+    <hyperlink ref="E18" r:id="rId15"/>
+    <hyperlink ref="E19" r:id="rId16"/>
+    <hyperlink ref="E20" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>